<commit_message>
added url normalisation strategy to source page
</commit_message>
<xml_diff>
--- a/na-service/src/test/resources/func/parser/source/Categories.xlsx
+++ b/na-service/src/test/resources/func/parser/source/Categories.xlsx
@@ -11,17 +11,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="73">
   <si>
     <t>name</t>
   </si>
   <si>
+    <t>type</t>
+  </si>
+  <si>
     <t>parent</t>
   </si>
   <si>
     <t>World</t>
   </si>
   <si>
+    <t>REGION</t>
+  </si>
+  <si>
     <t>Asia</t>
   </si>
   <si>
@@ -37,6 +43,12 @@
     <t>America</t>
   </si>
   <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Latin</t>
+  </si>
+  <si>
     <t>Africa</t>
   </si>
   <si>
@@ -52,9 +64,18 @@
     <t>Russia</t>
   </si>
   <si>
+    <t>England</t>
+  </si>
+  <si>
+    <t>Belarus</t>
+  </si>
+  <si>
     <t>Startup</t>
   </si>
   <si>
+    <t>COMMON</t>
+  </si>
+  <si>
     <t>Personal</t>
   </si>
   <si>
@@ -142,44 +163,80 @@
     <t>Breaking</t>
   </si>
   <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>Ecology</t>
+  </si>
+  <si>
+    <t>Lifestyle</t>
+  </si>
+  <si>
+    <t>Arts</t>
+  </si>
+  <si>
+    <t>Photo</t>
+  </si>
+  <si>
+    <t>Movies</t>
+  </si>
+  <si>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Digital</t>
+  </si>
+  <si>
+    <t>Exhibition</t>
+  </si>
+  <si>
+    <t>Graphic Design</t>
+  </si>
+  <si>
+    <t>Sports</t>
+  </si>
+  <si>
+    <t>Travel</t>
+  </si>
+  <si>
+    <t>Space</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
     <t>Retirement</t>
   </si>
   <si>
-    <t>Management</t>
-  </si>
-  <si>
-    <t>Ecology</t>
-  </si>
-  <si>
-    <t>Lifestyle</t>
-  </si>
-  <si>
-    <t>Arts</t>
-  </si>
-  <si>
-    <t>Photo</t>
-  </si>
-  <si>
-    <t>Architecture</t>
-  </si>
-  <si>
-    <t>Design</t>
-  </si>
-  <si>
-    <t>Digital</t>
-  </si>
-  <si>
-    <t>Exhibition</t>
-  </si>
-  <si>
-    <t>Graphic Design</t>
+    <t>Football</t>
+  </si>
+  <si>
+    <t>Yoga</t>
+  </si>
+  <si>
+    <t>Cars</t>
+  </si>
+  <si>
+    <t>Cooking</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Music</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -189,7 +246,6 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <sz val="13.0"/>
       <color theme="1"/>
@@ -210,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -218,9 +274,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -446,380 +499,706 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>2</v>
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="s">
-        <v>16</v>
+      <c r="A16" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C17" s="1"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="1"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>18</v>
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>18</v>
+      <c r="A24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>25</v>
+      <c r="A38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>39</v>
+        <v>20</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>21</v>
+        <v>48</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="3" t="s">
-        <v>46</v>
+      <c r="A47" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>47</v>
+        <v>28</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="s">
-        <v>49</v>
+      <c r="A50" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="2" t="s">
-        <v>50</v>
+      <c r="A51" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>47</v>
+      <c r="A52" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>47</v>
+      <c r="A53" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>47</v>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactored parsing with multiple strategies
</commit_message>
<xml_diff>
--- a/na-service/src/test/resources/func/parser/source/Categories.xlsx
+++ b/na-service/src/test/resources/func/parser/source/Categories.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="87">
   <si>
     <t>name</t>
   </si>
@@ -109,48 +109,48 @@
     <t>Programming</t>
   </si>
   <si>
+    <t>Economics</t>
+  </si>
+  <si>
+    <t>Woman</t>
+  </si>
+  <si>
+    <t>Investing</t>
+  </si>
+  <si>
+    <t>Markets</t>
+  </si>
+  <si>
+    <t>Trading</t>
+  </si>
+  <si>
+    <t>Stock Market</t>
+  </si>
+  <si>
+    <t>Online Shopping</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Money</t>
+  </si>
+  <si>
+    <t>Crypto</t>
+  </si>
+  <si>
+    <t>Stocks</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Freelance</t>
+  </si>
+  <si>
     <t>Business</t>
   </si>
   <si>
-    <t>Woman</t>
-  </si>
-  <si>
-    <t>Investing</t>
-  </si>
-  <si>
-    <t>Markets</t>
-  </si>
-  <si>
-    <t>Trading</t>
-  </si>
-  <si>
-    <t>Stock Market</t>
-  </si>
-  <si>
-    <t>Online Shopping</t>
-  </si>
-  <si>
-    <t>Finance</t>
-  </si>
-  <si>
-    <t>Money</t>
-  </si>
-  <si>
-    <t>Crypto</t>
-  </si>
-  <si>
-    <t>Stocks</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>Freelance</t>
-  </si>
-  <si>
-    <t>Small Business</t>
-  </si>
-  <si>
     <t>Social Media</t>
   </si>
   <si>
@@ -172,7 +172,7 @@
     <t>Lifestyle</t>
   </si>
   <si>
-    <t>Arts</t>
+    <t>Culture</t>
   </si>
   <si>
     <t>Photo</t>
@@ -230,6 +230,48 @@
   </si>
   <si>
     <t>Music</t>
+  </si>
+  <si>
+    <t>Theatre</t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Animals</t>
   </si>
 </sst>
 </file>
@@ -1201,6 +1243,157 @@
         <v>53</v>
       </c>
     </row>
+    <row r="71">
+      <c r="A71" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added HTML_TAG parsing support added Bangkok Post to test data
</commit_message>
<xml_diff>
--- a/na-service/src/test/resources/func/parser/source/Categories.xlsx
+++ b/na-service/src/test/resources/func/parser/source/Categories.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="88">
   <si>
     <t>name</t>
   </si>
@@ -124,9 +124,6 @@
     <t>Trading</t>
   </si>
   <si>
-    <t>Stock Market</t>
-  </si>
-  <si>
     <t>Online Shopping</t>
   </si>
   <si>
@@ -272,6 +269,12 @@
   </si>
   <si>
     <t>Animals</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>Thailand</t>
   </si>
 </sst>
 </file>
@@ -916,7 +919,7 @@
         <v>20</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38">
@@ -927,7 +930,7 @@
         <v>20</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39">
@@ -937,9 +940,6 @@
       <c r="B39" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
@@ -970,9 +970,6 @@
       <c r="B42" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
@@ -981,6 +978,9 @@
       <c r="B43" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="C43" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
@@ -989,9 +989,6 @@
       <c r="B44" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
@@ -1011,7 +1008,7 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>20</v>
@@ -1019,14 +1016,14 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -1034,7 +1031,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -1048,6 +1045,9 @@
       <c r="B51" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="C51" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
@@ -1057,7 +1057,7 @@
         <v>20</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53">
@@ -1068,7 +1068,7 @@
         <v>20</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54">
@@ -1079,7 +1079,7 @@
         <v>20</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55">
@@ -1090,7 +1090,7 @@
         <v>20</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56">
@@ -1101,7 +1101,7 @@
         <v>20</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57">
@@ -1112,7 +1112,7 @@
         <v>20</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58">
@@ -1122,9 +1122,6 @@
       <c r="B58" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
@@ -1149,6 +1146,9 @@
       <c r="B61" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="C61" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
@@ -1157,9 +1157,6 @@
       <c r="B62" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
@@ -1168,6 +1165,9 @@
       <c r="B63" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="C63" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
@@ -1177,7 +1177,7 @@
         <v>20</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65">
@@ -1188,7 +1188,7 @@
         <v>20</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66">
@@ -1199,7 +1199,7 @@
         <v>20</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
     </row>
     <row r="67">
@@ -1209,16 +1209,16 @@
       <c r="B67" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="69">
@@ -1226,10 +1226,10 @@
         <v>71</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
     </row>
     <row r="70">
@@ -1240,7 +1240,7 @@
         <v>20</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="71">
@@ -1250,9 +1250,6 @@
       <c r="B71" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
@@ -1261,16 +1258,19 @@
       <c r="B72" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="C72" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74">
@@ -1377,10 +1377,10 @@
         <v>85</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
     </row>
     <row r="84">
@@ -1391,7 +1391,18 @@
         <v>20</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>